<commit_message>
Linked Ui and Controls Added function for graph update and plotting test recipe preview
</commit_message>
<xml_diff>
--- a/Example_Test_Recipe.xlsx
+++ b/Example_Test_Recipe.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gd903\School\Senior Design\Team-108-Generation-of-Synthetic-Battery-Gas-for-Fire-and-Explosion-Testing-\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Devin\School\Senior Design\Team-108-Generation-of-Synthetic-Battery-Gas-for-Fire-and-Explosion-Testing-\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C7886685-6762-4348-8330-1904460255B2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D14C9C86-43FD-41C9-BB7E-C9BCD4183288}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="11424" yWindow="0" windowWidth="11712" windowHeight="13776" xr2:uid="{2CE868BB-4CDE-422B-A877-E4D21E68C372}"/>
+    <workbookView xWindow="4245" yWindow="4245" windowWidth="28800" windowHeight="15345" xr2:uid="{2CE868BB-4CDE-422B-A877-E4D21E68C372}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -53,10 +53,10 @@
     <t>O2</t>
   </si>
   <si>
-    <t>Time (s)</t>
+    <t>Heat Release Rate (kW)</t>
   </si>
   <si>
-    <t>Heat Release Rate (kW)</t>
+    <t>Time (s)</t>
   </si>
 </sst>
 </file>
@@ -430,18 +430,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1205A373-0027-4370-B8D0-F88183E8D924}">
   <dimension ref="A1:G16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G19" sqref="G19"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="7" max="7" width="19.88671875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="19.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B1" t="s">
         <v>0</v>
@@ -459,10 +457,10 @@
         <v>3</v>
       </c>
       <c r="G1" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>0</v>
       </c>
@@ -485,7 +483,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>1</v>
       </c>
@@ -508,7 +506,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>2</v>
       </c>
@@ -531,7 +529,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>3</v>
       </c>
@@ -554,7 +552,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>4</v>
       </c>
@@ -577,7 +575,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>5</v>
       </c>
@@ -600,7 +598,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>6</v>
       </c>
@@ -623,7 +621,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>7</v>
       </c>
@@ -646,7 +644,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>8</v>
       </c>
@@ -669,7 +667,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>9</v>
       </c>
@@ -692,7 +690,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>10</v>
       </c>
@@ -715,7 +713,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>11</v>
       </c>
@@ -738,7 +736,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>13</v>
       </c>
@@ -761,7 +759,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>15</v>
       </c>
@@ -784,7 +782,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>17</v>
       </c>

</xml_diff>